<commit_message>
feat: Completed and submitted PROG2113 Module 11 MC-FTE
</commit_message>
<xml_diff>
--- a/Courses/PROG2113 - HTML and CSS/Modules/Module 10 - Web Development/Assignments/Test_Plan_Completed.xlsx
+++ b/Courses/PROG2113 - HTML and CSS/Modules/Module 10 - Web Development/Assignments/Test_Plan_Completed.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="73">
   <si>
     <t>Web Page Document Test Plan</t>
   </si>
@@ -245,6 +245,11 @@
   </si>
   <si>
     <t xml:space="preserve"> T1/DS1 (1.544Mbps)</t>
+  </si>
+  <si>
+    <t>All responsiveness very good.  This is, of course, a very limited website.  
+Still finding the colors kind of plain.  Should convert to white background with very crisp images and so that they pop when a client opens them.  
+There really isn't anything here that would slow down the website . . . so it this site were used in say Bali or Saudi Arabia, it would still come up just as fast as in the US.</t>
   </si>
 </sst>
 </file>
@@ -784,7 +789,7 @@
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="23" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="25" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1896,7 +1901,9 @@
       <c r="N30" s="52"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="53"/>
+      <c r="A31" s="53" t="s">
+        <v>72</v>
+      </c>
       <c r="B31" s="54"/>
       <c r="C31" s="54"/>
       <c r="D31" s="54"/>

</xml_diff>